<commit_message>
Added stub for post, TestNG test
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20351"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F4ED61-24BF-4ECD-9A33-66E73B795B34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -31,21 +30,6 @@
     <t>/foo/bar/hello</t>
   </si>
   <si>
-    <t>/servicedelivery/102</t>
-  </si>
-  <si>
-    <t>/servicedelivery/103</t>
-  </si>
-  <si>
-    <t>{"foo", "bar"}</t>
-  </si>
-  <si>
-    <t>{"servicedelivery", "102"}</t>
-  </si>
-  <si>
-    <t>{"servicedelivery", "103"}</t>
-  </si>
-  <si>
     <t>Method</t>
   </si>
   <si>
@@ -58,16 +42,37 @@
     <t>StatusCode</t>
   </si>
   <si>
-    <t>{"servicedelivery", "101"}</t>
-  </si>
-  <si>
-    <t>/servicedelivery/101</t>
+    <t>{"foo" : "bar"}</t>
+  </si>
+  <si>
+    <t>/serviceDelivery/101</t>
+  </si>
+  <si>
+    <t>{"serviceDelivery" : "101"}</t>
+  </si>
+  <si>
+    <t>/serviceDelivery/102</t>
+  </si>
+  <si>
+    <t>{"serviceDelivery" : "102"}</t>
+  </si>
+  <si>
+    <t>/serviceDelivery/103</t>
+  </si>
+  <si>
+    <t>{"serviceDelivery" : "103"}</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/serviceDelivery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -381,11 +386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985FBD0B-0097-43C7-8862-887B9A251226}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,16 +406,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -424,7 +429,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>200</v>
@@ -438,10 +443,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>200</v>
@@ -455,10 +460,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E4">
         <v>200</v>
@@ -472,17 +477,32 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>